<commit_message>
joy 07 26 2017
</commit_message>
<xml_diff>
--- a/_Rmd/data/ehs mar 2017.xlsx
+++ b/_Rmd/data/ehs mar 2017.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="25">
   <si>
     <t>date</t>
   </si>
@@ -426,13 +426,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M221"/>
+  <dimension ref="A1:M223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B202" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B206" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F221" sqref="F221"/>
+      <selection pane="bottomRight" activeCell="E224" sqref="E224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -8686,16 +8686,13 @@
         <v>2017</v>
       </c>
       <c r="C221">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D221" t="s">
         <v>14</v>
       </c>
       <c r="E221">
         <v>4</v>
-      </c>
-      <c r="F221">
-        <v>54</v>
       </c>
       <c r="H221">
         <v>569</v>
@@ -8710,6 +8707,40 @@
       <c r="K221">
         <f t="shared" si="16"/>
         <v>643.87373709883104</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A222" s="1">
+        <v>42856</v>
+      </c>
+      <c r="B222">
+        <v>2017</v>
+      </c>
+      <c r="C222">
+        <v>555</v>
+      </c>
+      <c r="D222" t="s">
+        <v>15</v>
+      </c>
+      <c r="E222">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A223" s="1">
+        <v>42887</v>
+      </c>
+      <c r="B223">
+        <v>2017</v>
+      </c>
+      <c r="C223">
+        <v>601</v>
+      </c>
+      <c r="D223" t="s">
+        <v>16</v>
+      </c>
+      <c r="E223">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>